<commit_message>
fixed issue of checking if pathology is present (always check with lowercase)
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ErrorFiles/dementia_Niguarda_v1.xlsx
+++ b/src/main/resources/data/ErrorFiles/dementia_Niguarda_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="135">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -76,9 +76,6 @@
     <t xml:space="preserve">Patient ID</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/ID_UNI_PAZIENTE</t>
-  </si>
-  <si>
     <t xml:space="preserve">SESSO</t>
   </si>
   <si>
@@ -109,10 +106,7 @@
     <t xml:space="preserve">Date of Birth</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/ID_UNI_NOSOLOGICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[DATA_INIZIO – DATA_NASCITA keep only years], [DATA_INIZIO-DATA_NASCITA keep only months left], [(DATA_INIZIO-DATA_NASCITA) corresponds to one of the groups: {“-50y”},{”50-59y”},{”60-69y”},{”70-79y”},{”+80y”}]</t>
+    <t xml:space="preserve">[stays the same], [(CurrentDate-AGE)*12], [(CurrentDate-AGE) corresponds to one of the groups: {“-50y”},{”50-59y”},{”60-69y”},{”70-79y”},{”+80y”}]</t>
   </si>
   <si>
     <t xml:space="preserve">subjectageyears, subjectage, agegroup</t>
@@ -136,7 +130,7 @@
     <t xml:space="preserve">Hospital treatment code (ICD9) for the MRI</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/CODICE_PRESTAZIONE_ICD9</t>
+    <t xml:space="preserve">/root/treatment/CODICE_PRESTAZIONE_ICD9</t>
   </si>
   <si>
     <t xml:space="preserve">HANDEDNESS</t>
@@ -166,7 +160,7 @@
     <t xml:space="preserve">Years of Education</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/demographics/EDUCATION</t>
+    <t xml:space="preserve">/root/demographics/EDUCATION</t>
   </si>
   <si>
     <t xml:space="preserve">PROFILO_CLINICO</t>
@@ -175,7 +169,7 @@
     <t xml:space="preserve">DIAGNOSIS CATEGORY</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/diagnosis/PROFILO_CLINICO</t>
+    <t xml:space="preserve">/root/diagnosis/PROFILO_CLINICO</t>
   </si>
   <si>
     <t xml:space="preserve">MMSE_SCORE</t>
@@ -193,7 +187,7 @@
     <t xml:space="preserve">MMSE subscore for orientation to time</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/ORIENTATION_TO_TIME</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/ORIENTATION_TO_TIME</t>
   </si>
   <si>
     <t xml:space="preserve">ORIENTATION_TO_PLACE</t>
@@ -202,7 +196,7 @@
     <t xml:space="preserve">MMSE subscore for orientation to place</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/ORIENTATION_TO_PLACE</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/ORIENTATION_TO_PLACE</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTRATION</t>
@@ -211,7 +205,7 @@
     <t xml:space="preserve">MMSE subscore for registration</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/REGISTRATION</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/REGISTRATION</t>
   </si>
   <si>
     <t xml:space="preserve">CALCULATION</t>
@@ -220,7 +214,7 @@
     <t xml:space="preserve">MMSE subscore for calculation</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/CALCULATION</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/CALCULATION</t>
   </si>
   <si>
     <t xml:space="preserve">ATTENTION</t>
@@ -229,7 +223,7 @@
     <t xml:space="preserve">MMSE subscore for attention</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/ATTENTION</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/ATTENTION</t>
   </si>
   <si>
     <t xml:space="preserve">RECALL</t>
@@ -238,7 +232,7 @@
     <t xml:space="preserve">MMSE subscore for recall</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/RECALL</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/RECALL</t>
   </si>
   <si>
     <t xml:space="preserve">LANGUAGE</t>
@@ -247,7 +241,7 @@
     <t xml:space="preserve">MMSE subscore for language</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/LANGUAGE</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/LANGUAGE</t>
   </si>
   <si>
     <t xml:space="preserve">REPETITION</t>
@@ -256,7 +250,7 @@
     <t xml:space="preserve">MMSE subscore for repetition</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/REPETITION</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/REPETITION</t>
   </si>
   <si>
     <t xml:space="preserve">STAGE_COMMANDS_3  </t>
@@ -268,7 +262,7 @@
     <t xml:space="preserve">MMSE subscore for complex commands</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/STAGE_COMMANDS_3</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/STAGE_COMMANDS_3</t>
   </si>
   <si>
     <t xml:space="preserve">READ_AND_OBEY</t>
@@ -277,7 +271,7 @@
     <t xml:space="preserve">MMSE subscore for read and obey</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/READ_AND_OBEY</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/READ_AND_OBEY</t>
   </si>
   <si>
     <t xml:space="preserve">SENTENCE</t>
@@ -286,7 +280,7 @@
     <t xml:space="preserve">MMSE subscore for sentence</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/SENTENCE</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/SENTENCE</t>
   </si>
   <si>
     <t xml:space="preserve">PRAXIA</t>
@@ -295,7 +289,7 @@
     <t xml:space="preserve">MMSE subscore for praxia</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/neuropsychology/mmse/PRAXIA</t>
+    <t xml:space="preserve">/root/neuropsychology/mmse/PRAXIA</t>
   </si>
   <si>
     <t xml:space="preserve">Episode</t>
@@ -307,7 +301,7 @@
     <t xml:space="preserve">Clinical episode start date</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/DATA_INIZIO</t>
+    <t xml:space="preserve">/root/treatment/DATA_INIZIO</t>
   </si>
   <si>
     <t xml:space="preserve">DATA_FINE</t>
@@ -316,7 +310,7 @@
     <t xml:space="preserve">Clinical episode end date</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/DATA_FINE</t>
+    <t xml:space="preserve">/root/treatment/DATA_FINE</t>
   </si>
   <si>
     <t xml:space="preserve">REGIME</t>
@@ -328,7 +322,7 @@
     <t xml:space="preserve">Way to perform hospitalization ( 1 =inpatient surgery; 2=day hospital; 4= MAC; 5= anticipato).</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/REGIME</t>
+    <t xml:space="preserve">/root/treatment/REGIME</t>
   </si>
   <si>
     <t xml:space="preserve">REPARTO_INIZIO</t>
@@ -337,7 +331,7 @@
     <t xml:space="preserve">Start ward (only for inpatients)</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/REPARTO_INIZIO</t>
+    <t xml:space="preserve">/root/treatment/REPARTO_INIZIO</t>
   </si>
   <si>
     <t xml:space="preserve">REPARTO_FINE</t>
@@ -346,7 +340,7 @@
     <t xml:space="preserve">End ward (only for inpatients)</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/REPARTO_FINE</t>
+    <t xml:space="preserve">/root/treatment/REPARTO_FINE</t>
   </si>
   <si>
     <t xml:space="preserve">COD_DIAGNOSI_ICD9</t>
@@ -355,7 +349,7 @@
     <t xml:space="preserve">Diagnosis only from emergency episode</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/diagnosis/COD_DIAGNOSI_ICD9</t>
+    <t xml:space="preserve">/root/diagnosis/COD_DIAGNOSI_ICD9</t>
   </si>
   <si>
     <t xml:space="preserve">CODICE_DIAGNOSI_1_ICD9</t>
@@ -364,7 +358,7 @@
     <t xml:space="preserve">First diagnosis code from inpatient episode</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/diagnosis/</t>
+    <t xml:space="preserve">/root/diagnosis/</t>
   </si>
   <si>
     <t xml:space="preserve">CODICE_DIAGNOSI_2_ICD9</t>
@@ -406,7 +400,7 @@
     <t xml:space="preserve">Episode type (“I” = inpatient; “U” =emergency; “E” = outpatient)</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/treatment/</t>
+    <t xml:space="preserve">/root/treatment/</t>
   </si>
   <si>
     <t xml:space="preserve">Imaging</t>
@@ -421,25 +415,16 @@
     <t xml:space="preserve">PACS Accession number for the MRI</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/ACCESSION_NUMBER</t>
-  </si>
-  <si>
     <t xml:space="preserve">DATA_ESAME</t>
   </si>
   <si>
     <t xml:space="preserve">Exam date (date of the MRI)</t>
   </si>
   <si>
-    <t xml:space="preserve">/dementia/DATA_ESAME</t>
-  </si>
-  <si>
     <t xml:space="preserve">RICHIEDENTE</t>
   </si>
   <si>
     <t xml:space="preserve">Ward applying the exam. “3760 Neurologia Degenza” is Neuroscience ward. Please convert every other value to null or blank.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/dementia/RICHIEDENTE</t>
   </si>
 </sst>
 </file>
@@ -449,12 +434,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -489,6 +473,12 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -571,11 +561,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -583,19 +581,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -618,13 +608,13 @@
   </sheetPr>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,9 +680,7 @@
         <v>17</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
@@ -702,32 +690,32 @@
         <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,46 +723,44 @@
         <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="5"/>
-      <c r="J4" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -782,40 +768,38 @@
         <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -823,65 +807,65 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -889,28 +873,28 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -918,13 +902,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>15</v>
@@ -932,30 +916,30 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>15</v>
@@ -963,14 +947,14 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -978,13 +962,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>15</v>
@@ -992,14 +976,14 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -1007,13 +991,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>15</v>
@@ -1021,14 +1005,14 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -1036,13 +1020,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
@@ -1050,14 +1034,14 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -1065,13 +1049,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>15</v>
@@ -1079,14 +1063,14 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -1094,13 +1078,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>15</v>
@@ -1108,14 +1092,14 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -1123,13 +1107,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>15</v>
@@ -1137,14 +1121,14 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -1152,13 +1136,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>15</v>
@@ -1166,14 +1150,14 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -1181,13 +1165,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>15</v>
@@ -1195,14 +1179,14 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -1210,13 +1194,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>15</v>
@@ -1224,14 +1208,14 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
@@ -1239,13 +1223,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>15</v>
@@ -1253,14 +1237,14 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -1268,13 +1252,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>15</v>
@@ -1282,14 +1266,14 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
@@ -1297,28 +1281,28 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -1326,28 +1310,28 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -1355,30 +1339,30 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -1386,28 +1370,28 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
@@ -1415,28 +1399,28 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
@@ -1444,28 +1428,28 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -1473,28 +1457,28 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
@@ -1502,28 +1486,28 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
@@ -1531,28 +1515,28 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
@@ -1560,28 +1544,28 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
@@ -1589,28 +1573,28 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -1618,28 +1602,28 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
@@ -1647,30 +1631,30 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
@@ -1678,16 +1662,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -1695,70 +1679,64 @@
         <v>16</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I36" s="7"/>
-      <c r="J36" s="7" t="s">
-        <v>133</v>
-      </c>
+      <c r="J36" s="7"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I37" s="7"/>
-      <c r="J37" s="7" t="s">
-        <v>136</v>
-      </c>
+      <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I38" s="7"/>
-      <c r="J38" s="7" t="s">
-        <v>139</v>
-      </c>
+      <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
@@ -1766,7 +1744,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>